<commit_message>
small changes for partial match
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_UT_SS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="68">
   <si>
     <t>VIN</t>
   </si>
@@ -200,21 +200,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Volkswagen</t>
-  </si>
-  <si>
-    <t>Arteon</t>
-  </si>
-  <si>
-    <t>Arteon SEL</t>
-  </si>
-  <si>
-    <t>Coupe</t>
-  </si>
-  <si>
-    <t>Sedan</t>
-  </si>
-  <si>
     <t>8L V12</t>
   </si>
   <si>
@@ -234,13 +219,22 @@
   </si>
   <si>
     <t>7MSRP17H&amp;V</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN</t>
+  </si>
+  <si>
+    <t>GOLF</t>
+  </si>
+  <si>
+    <t>HATCHBACK 4 DOOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,8 +256,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.4"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +273,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -289,11 +295,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -579,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,7 +601,10 @@
     <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.5546875" customWidth="1"/>
     <col min="15" max="15" width="18.77734375" customWidth="1"/>
     <col min="21" max="21" width="22.88671875" customWidth="1"/>
@@ -1184,27 +1199,27 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="3">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H6" s="3">
         <v>88888</v>
@@ -1213,19 +1228,19 @@
         <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="O6" s="3">
         <v>12</v>
@@ -1237,7 +1252,7 @@
         <v>214</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="S6" s="3">
         <v>4</v>
@@ -1261,12 +1276,12 @@
         <v>37</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA6" s="3">
+        <v>60</v>
+      </c>
+      <c r="AA6" s="5">
         <v>35</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AB6" s="5">
         <v>44</v>
       </c>
       <c r="AC6" s="3" t="s">
@@ -1276,16 +1291,16 @@
         <v>39</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="AG6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AI6" s="3">
         <v>20000101</v>

</xml_diff>

<commit_message>
PAS-760: Changed doc name
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_UT_SS.xlsx
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,7 +862,7 @@
         <v>38</v>
       </c>
       <c r="AI2" s="3">
-        <v>20150101</v>
+        <v>20000101</v>
       </c>
       <c r="AJ2" s="3" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
PAS-6576 fixed TestVinUpload newVinAdded test (link to testData was wrong), fixed Excel file to match the test
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_UT_SS.xlsx
@@ -627,7 +627,7 @@
   <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,16 +862,16 @@
         <v>39</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="AI2" s="3">
         <v>20010101</v>
@@ -1094,16 +1094,16 @@
         <v>39</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="AI4" s="3">
         <v>20150101</v>

</xml_diff>